<commit_message>
redundant drive upload code
</commit_message>
<xml_diff>
--- a/template (4).xlsx
+++ b/template (4).xlsx
@@ -17123,7 +17123,7 @@
       </c>
       <c r="B1008" t="inlineStr">
         <is>
-          <t>Seamless Pattern</t>
+          <t>Digital Paper</t>
         </is>
       </c>
       <c r="C1008" t="inlineStr">
@@ -17133,12 +17133,12 @@
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>Cherry Blossoms</t>
+          <t>2nd Digital Paper</t>
         </is>
       </c>
       <c r="E1008" t="inlineStr">
         <is>
-          <t>['A luxurious modern living room with floor-to-ceiling windows, natural light streaming in, minimalist white furniture, warm wood accents, and a statement chandelier. Soft textiles, potted plants, and abstract art create a sophisticated atmosphere. Photorealistic, interior design photography --ar 1:1 --v 5.2']</t>
+          <t>['An elegant open-concept kitchen with marble countertops, brass fixtures, and custom white cabinetry. Island with pendant lights, herringbone wood floors, and professional appliances. Bright and airy with modern farmhouse touches. Architectural photography style --ar 1:1 --v 5.2']</t>
         </is>
       </c>
       <c r="I1008" t="inlineStr"/>

</xml_diff>

<commit_message>
drive links & raw sub-folder
</commit_message>
<xml_diff>
--- a/template (4).xlsx
+++ b/template (4).xlsx
@@ -733,14 +733,48 @@
       <c r="M5" s="6" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="6" t="n"/>
-      <c r="F6" s="6" t="n"/>
-      <c r="G6" s="6" t="n"/>
-      <c r="H6" s="6" t="n"/>
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Watercolor</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Marbleized Patterns</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>High-resolution digital paper texture with soft marbleized watercolor design, smooth background, detailed intricate surface, soft texture intensity --v 6.1</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>/Users/mac/Documents/git/midjourney/Digital Paper Store/Digital Paper Store - Raw Folder/Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>/Users/mac/Documents/git/midjourney/Digital Paper Store/Digital Paper Store - Digital Paper/Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?id=1D7bJtRQsi6VohnqpVhXiF087EMTsa0g3
+https://drive.google.com/uc?id=1-T76_I4-3vUBkRcviSruFalwU_39FAxF
+https://drive.google.com/uc?id=17tLohqddwPzWiLYzgOqC1gMao9FTDOdM</t>
+        </is>
+      </c>
+      <c r="H6" s="6" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1uLMHtCBAc1SbojifbErp34KTsGjC3i_L?usp=sharing</t>
+        </is>
+      </c>
       <c r="I6" s="6" t="n"/>
       <c r="J6" s="6" t="n"/>
       <c r="K6" s="6" t="n"/>
@@ -748,13 +782,41 @@
       <c r="M6" s="6" t="n"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="6" t="n"/>
-      <c r="F7" s="6" t="n"/>
-      <c r="G7" s="6" t="n"/>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Watercolor</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Marbleized Patterns</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>High-resolution digital paper texture with soft marbleized watercolor design, smooth background, detailed intricate surface, soft texture intensity --v 6.1</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>/Users/mac/Documents/git/midjourney/Digital Paper Store/Digital Paper Store - Raw Folder/Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>/Users/mac/Documents/git/midjourney/Digital Paper Store/Digital Paper Store - Digital Paper/Marbleized Patterns - Watercolor - Digital Paper</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/drive/folders/1uLMHtCBAc1SbojifbErp34KTsGjC3i_L?usp=sharing</t>
+        </is>
+      </c>
       <c r="H7" s="6" t="n"/>
       <c r="I7" s="6" t="n"/>
       <c r="J7" s="6" t="n"/>

</xml_diff>